<commit_message>
Downloading Virtual Machine Image
</commit_message>
<xml_diff>
--- a/1.Installing-VMware-and-VirtualBox-on-Windows/1.Software_Download_Installation.xlsx
+++ b/1.Installing-VMware-and-VirtualBox-on-Windows/1.Software_Download_Installation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quang\oracle\1.Installing-VMware-and-VirtualBox-on-Windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C413F1CB-7FFA-4DAA-B1D1-FD7FCB338957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79490140-48B7-4DEF-9C07-6C9193B00FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="315" windowWidth="26205" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28965" yWindow="315" windowWidth="26205" windowHeight="13365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstallingVMwareAndVirtualBox" sheetId="1" r:id="rId1"/>
+    <sheet name="DownloadingVirtualMachineImage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Installing VMware and VirtualBox on Windows</t>
     <phoneticPr fontId="1"/>
@@ -48,6 +49,14 @@
   </si>
   <si>
     <t>https://www.virtualbox.org/wiki/Downloads</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Downloading Virtual Machine Image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>download oracle pre-built virtual machine</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1053,6 +1062,143 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>127388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5764C5B6-AB0A-2FDD-5CA7-DB0F246D030E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752474" y="762000"/>
+          <a:ext cx="12030075" cy="4394588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>345500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB27F03A-81A1-3061-5359-057155CF82C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="815975" y="5334000"/>
+          <a:ext cx="12016800" cy="5210175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158749</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>442096</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322F821C-7599-13D1-25F6-532799201612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="815974" y="10826750"/>
+          <a:ext cx="12113397" cy="6022975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1318,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView topLeftCell="A469" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="B459" sqref="B459"/>
     </sheetView>
   </sheetViews>
@@ -2536,4 +2682,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32292DA1-BC4E-41D4-96C0-65238A30423A}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>